<commit_message>
Update PLANTILLA DE CARGA_ISR100_ENERO.xlsx
</commit_message>
<xml_diff>
--- a/PDRMYE/PRUEBAS/Plantillas_participaciones/PLANTILLA DE CARGA_ISR100_ENERO.xlsx
+++ b/PDRMYE/PRUEBAS/Plantillas_participaciones/PLANTILLA DE CARGA_ISR100_ENERO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Infinite\Desktop\Plantillas_participaciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Infinite\Documents\GITHUB\All-documents\PDRMYE\PRUEBAS\Plantillas_participaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -235,10 +235,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -353,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="37" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -367,25 +366,25 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Millares 2" xfId="1"/>
@@ -672,7 +671,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -686,19 +685,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -849,7 +848,7 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>40854</v>
       </c>
     </row>
@@ -866,7 +865,7 @@
       <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>958453</v>
       </c>
     </row>
@@ -951,7 +950,7 @@
       <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>200022</v>
       </c>
     </row>
@@ -983,7 +982,7 @@
       <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="11">
         <v>63037</v>
       </c>
     </row>
@@ -1034,7 +1033,7 @@
       <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="22">
         <v>1962822</v>
       </c>
     </row>
@@ -1153,7 +1152,7 @@
       <c r="D28" s="1">
         <v>1</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="12">
         <v>84063</v>
       </c>
     </row>
@@ -1187,7 +1186,7 @@
       <c r="D30" s="1">
         <v>1</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="13">
         <v>38338</v>
       </c>
     </row>
@@ -1238,7 +1237,7 @@
       <c r="D33" s="1">
         <v>1</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="14">
         <v>2717924</v>
       </c>
     </row>
@@ -1272,7 +1271,7 @@
       <c r="D35" s="1">
         <v>1</v>
       </c>
-      <c r="E35" s="16">
+      <c r="E35" s="15">
         <v>311132</v>
       </c>
     </row>
@@ -1289,7 +1288,7 @@
       <c r="D36" s="1">
         <v>1</v>
       </c>
-      <c r="E36" s="17">
+      <c r="E36" s="16">
         <v>42876</v>
       </c>
     </row>
@@ -1306,7 +1305,7 @@
       <c r="D37" s="1">
         <v>1</v>
       </c>
-      <c r="E37" s="18">
+      <c r="E37" s="17">
         <v>39981</v>
       </c>
     </row>
@@ -1374,7 +1373,7 @@
       <c r="D41" s="1">
         <v>1</v>
       </c>
-      <c r="E41" s="19">
+      <c r="E41" s="18">
         <v>3463155</v>
       </c>
     </row>
@@ -1391,7 +1390,7 @@
       <c r="D42" s="1">
         <v>1</v>
       </c>
-      <c r="E42" s="20">
+      <c r="E42" s="19">
         <v>23184</v>
       </c>
     </row>
@@ -1408,7 +1407,7 @@
       <c r="D43" s="1">
         <v>1</v>
       </c>
-      <c r="E43" s="21">
+      <c r="E43" s="20">
         <v>287741</v>
       </c>
     </row>
@@ -1493,7 +1492,7 @@
       <c r="D48" s="1">
         <v>1</v>
       </c>
-      <c r="E48" s="22">
+      <c r="E48" s="21">
         <v>1022270</v>
       </c>
     </row>
@@ -1544,7 +1543,7 @@
       <c r="D51" s="1">
         <v>1</v>
       </c>
-      <c r="E51" s="24">
+      <c r="E51" s="23">
         <v>458011</v>
       </c>
     </row>

</xml_diff>